<commit_message>
ran allll the experiments
</commit_message>
<xml_diff>
--- a/Scripts/Python Script Versions/Experimental Data/Client Testing - multiple day pulls/Main Version12-13.xlsx
+++ b/Scripts/Python Script Versions/Experimental Data/Client Testing - multiple day pulls/Main Version12-13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Padmanie\Documents\GitHub\Capstone\DataCollection\Scripts\Python Script Versions\Experimental Data\Client Testing - multiple day pulls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389C4762-ABDE-4580-9892-31892D0485FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D39DA27-FDE5-4859-938D-0878AB6BC60E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hayden" sheetId="1" r:id="rId1"/>
@@ -1909,8 +1909,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2410,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>3</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>3</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>3</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>3</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>3</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>3</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>3</v>
       </c>
@@ -4495,6 +4495,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L61" xr:uid="{73BF7584-7A92-45AA-9BAC-25220B97EE6C}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="1">
       <filters>
         <filter val="0"/>
@@ -9779,8 +9784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5112AA-710D-4C34-B747-BD88046FB115}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>